<commit_message>
Added UI and functions for Archiving
</commit_message>
<xml_diff>
--- a/client/public/FinalUpload.xlsx
+++ b/client/public/FinalUpload.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nolimitmide/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nolimitmide/Desktop/tyu/client/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54A5AC6E-8AC4-3847-8F83-AA195EEBE2B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{347B50AD-2F0F-0943-AA49-5444F9E0B429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2560" yWindow="3740" windowWidth="27240" windowHeight="16440" xr2:uid="{6DA0F673-2ECF-594F-AADE-5450E617D137}"/>
   </bookViews>
@@ -472,19 +472,18 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="173.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -496,10 +495,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>

</xml_diff>